<commit_message>
finsihed self correction pipeline
</commit_message>
<xml_diff>
--- a/data/assess_hard_design.xlsx
+++ b/data/assess_hard_design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fhans/Documents/GenerativeBenchmarking/clone-anonymous-github/ChatGPT-Study-2757/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D0965-A60E-E142-9CF9-4825410F494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06768C7-EF51-1D4C-9A9E-04940F8862FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>